<commit_message>
Manuscript Updates and more PRISM data
</commit_message>
<xml_diff>
--- a/Processed Data/GIS/MonthlyPrecipPRISM.xlsx
+++ b/Processed Data/GIS/MonthlyPrecipPRISM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
   <si>
     <t>FID</t>
   </si>
@@ -127,6 +127,90 @@
   </si>
   <si>
     <t>Diff18</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>ppt_2_5003</t>
+  </si>
+  <si>
+    <t>ppt_2_5004</t>
+  </si>
+  <si>
+    <t>ppt_2_5005</t>
+  </si>
+  <si>
+    <t>ppt_2_5094</t>
+  </si>
+  <si>
+    <t>ppt_2_5095</t>
+  </si>
+  <si>
+    <t>ppt_2_5096</t>
+  </si>
+  <si>
+    <t>ppt_2_5097</t>
+  </si>
+  <si>
+    <t>ppt_2_5098</t>
+  </si>
+  <si>
+    <t>ppt_2_5099</t>
+  </si>
+  <si>
+    <t>ppt_2_5100</t>
+  </si>
+  <si>
+    <t>ppt_2_5101</t>
+  </si>
+  <si>
+    <t>ppt_2_5102</t>
+  </si>
+  <si>
+    <t>ppt_2_5103</t>
+  </si>
+  <si>
+    <t>ppt_2_5104</t>
+  </si>
+  <si>
+    <t>ppt_2_5105</t>
+  </si>
+  <si>
+    <t>ppt_2_5194</t>
+  </si>
+  <si>
+    <t>ppt_2_5195</t>
+  </si>
+  <si>
+    <t>ppt_2_5196</t>
+  </si>
+  <si>
+    <t>ppt_2_5197</t>
+  </si>
+  <si>
+    <t>ppt_2_5198</t>
+  </si>
+  <si>
+    <t>ppt_2_5199</t>
+  </si>
+  <si>
+    <t>ppt_2_5200</t>
+  </si>
+  <si>
+    <t>ppt_2_5201</t>
+  </si>
+  <si>
+    <t>ppt_2_5202</t>
+  </si>
+  <si>
+    <t>Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>WY2016</t>
   </si>
 </sst>
 </file>
@@ -1521,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG4"/>
+  <dimension ref="A1:BN9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AO4" sqref="AO4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,11 +1619,11 @@
     <col min="16" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.85546875" customWidth="1"/>
-    <col min="31" max="31" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.140625" customWidth="1"/>
     <col min="32" max="33" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1624,23 +1708,62 @@
       <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1">
+        <v>201510</v>
+      </c>
+      <c r="AD1">
+        <v>201511</v>
+      </c>
+      <c r="AE1">
+        <v>201512</v>
+      </c>
+      <c r="AF1">
+        <v>201601</v>
+      </c>
+      <c r="AG1">
+        <v>201602</v>
+      </c>
+      <c r="AH1">
+        <v>201603</v>
+      </c>
+      <c r="AI1">
+        <v>201604</v>
+      </c>
+      <c r="AJ1">
+        <v>201605</v>
+      </c>
+      <c r="AK1">
+        <v>201606</v>
+      </c>
+      <c r="AL1">
+        <v>201607</v>
+      </c>
+      <c r="AM1">
+        <v>201608</v>
+      </c>
+      <c r="AN1">
+        <v>201609</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP1" t="s">
         <v>31</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AQ1" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AR1" t="s">
         <v>33</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AS1" t="s">
         <v>34</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AT1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1726,26 +1849,66 @@
         <v>2.5399699</v>
       </c>
       <c r="AC2">
+        <v>50.877899999999997</v>
+      </c>
+      <c r="AD2">
+        <v>118.012</v>
+      </c>
+      <c r="AE2">
+        <v>205.17599999999999</v>
+      </c>
+      <c r="AF2">
+        <v>250.03700000000001</v>
+      </c>
+      <c r="AG2">
+        <v>57.329700000000003</v>
+      </c>
+      <c r="AH2">
+        <v>228.70699999999999</v>
+      </c>
+      <c r="AI2">
+        <v>75.908100000000005</v>
+      </c>
+      <c r="AJ2">
+        <v>31.494499999999999</v>
+      </c>
+      <c r="AK2">
+        <v>10.197699999999999</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>1.0299</v>
+      </c>
+      <c r="AO2">
+        <f>SUM(AC2:AN2)</f>
+        <v>1028.7698</v>
+      </c>
+      <c r="AP2">
         <f>SUM(E2:P2)</f>
         <v>2017.4938643000003</v>
       </c>
-      <c r="AD2">
+      <c r="AQ2">
         <f>SUM(Q2:AB2)</f>
         <v>796.96785289999991</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AR2" t="s">
         <v>32</v>
       </c>
-      <c r="AF2" s="1">
-        <f>AC2/AC3</f>
+      <c r="AS2" s="1">
+        <f>AP2/AP3</f>
         <v>1.353027510693618</v>
       </c>
-      <c r="AG2" s="1">
-        <f>AD2/AD3</f>
+      <c r="AT2" s="1">
+        <f>AQ2/AQ3</f>
         <v>1.1850249116484057</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1831,18 +1994,58 @@
         <v>10.4934998</v>
       </c>
       <c r="AC3">
+        <v>43.702300000000001</v>
+      </c>
+      <c r="AD3">
+        <v>112.086</v>
+      </c>
+      <c r="AE3">
+        <v>152.78</v>
+      </c>
+      <c r="AF3">
+        <v>204.16399999999999</v>
+      </c>
+      <c r="AG3">
+        <v>92.772999999999996</v>
+      </c>
+      <c r="AH3">
+        <v>141.74600000000001</v>
+      </c>
+      <c r="AI3">
+        <v>63.175800000000002</v>
+      </c>
+      <c r="AJ3">
+        <v>23.820900000000002</v>
+      </c>
+      <c r="AK3">
+        <v>6.8852900000000004</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0.54130800000000001</v>
+      </c>
+      <c r="AN3">
+        <v>1.2849699999999999</v>
+      </c>
+      <c r="AO3">
+        <f>SUM(AC3:AN3)</f>
+        <v>842.9595680000001</v>
+      </c>
+      <c r="AP3">
         <f>SUM(E3:P3)</f>
         <v>1491.0959668999999</v>
       </c>
-      <c r="AD3">
+      <c r="AQ3">
         <f>SUM(Q3:AB3)</f>
         <v>672.53257299999996</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AR3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
       <c r="E4" s="2">
         <v>42644</v>
       </c>
@@ -1914,6 +2117,807 @@
       </c>
       <c r="AB4" s="2">
         <v>43344</v>
+      </c>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+    </row>
+    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" t="s">
+        <v>16</v>
+      </c>
+      <c r="S6" t="s">
+        <v>17</v>
+      </c>
+      <c r="T6" t="s">
+        <v>18</v>
+      </c>
+      <c r="U6" t="s">
+        <v>19</v>
+      </c>
+      <c r="V6" t="s">
+        <v>20</v>
+      </c>
+      <c r="W6" t="s">
+        <v>21</v>
+      </c>
+      <c r="X6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>59</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC6">
+        <v>201510</v>
+      </c>
+      <c r="BD6">
+        <v>201511</v>
+      </c>
+      <c r="BE6">
+        <v>201512</v>
+      </c>
+      <c r="BF6">
+        <v>201601</v>
+      </c>
+      <c r="BG6">
+        <v>201602</v>
+      </c>
+      <c r="BH6">
+        <v>201603</v>
+      </c>
+      <c r="BI6">
+        <v>201604</v>
+      </c>
+      <c r="BJ6">
+        <v>201605</v>
+      </c>
+      <c r="BK6">
+        <v>201606</v>
+      </c>
+      <c r="BL6">
+        <v>201607</v>
+      </c>
+      <c r="BM6">
+        <v>201608</v>
+      </c>
+      <c r="BN6">
+        <v>201609</v>
+      </c>
+    </row>
+    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>-119.565696</v>
+      </c>
+      <c r="E7">
+        <v>37.675826999999998</v>
+      </c>
+      <c r="F7">
+        <v>159.96700000000001</v>
+      </c>
+      <c r="G7">
+        <v>69.757999999999996</v>
+      </c>
+      <c r="H7">
+        <v>242.91399999999999</v>
+      </c>
+      <c r="I7">
+        <v>712.11800000000005</v>
+      </c>
+      <c r="J7">
+        <v>492.29599999999999</v>
+      </c>
+      <c r="K7">
+        <v>106.33199999999999</v>
+      </c>
+      <c r="L7">
+        <v>170.44399999999999</v>
+      </c>
+      <c r="M7">
+        <v>11.5787</v>
+      </c>
+      <c r="N7">
+        <v>9.1510200000000008</v>
+      </c>
+      <c r="O7">
+        <v>1.5070999999999999E-2</v>
+      </c>
+      <c r="P7">
+        <v>11.130800000000001</v>
+      </c>
+      <c r="Q7">
+        <v>31.789300000000001</v>
+      </c>
+      <c r="R7">
+        <v>10.006500000000001</v>
+      </c>
+      <c r="S7">
+        <v>110.884</v>
+      </c>
+      <c r="T7">
+        <v>5.3028199999999996</v>
+      </c>
+      <c r="U7">
+        <v>117.038</v>
+      </c>
+      <c r="V7">
+        <v>29.012699999999999</v>
+      </c>
+      <c r="W7">
+        <v>415.17500000000001</v>
+      </c>
+      <c r="X7">
+        <v>89.858400000000003</v>
+      </c>
+      <c r="Y7">
+        <v>16.902799999999999</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0.247673</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>2.5399699999999998</v>
+      </c>
+      <c r="AD7">
+        <v>167.21600000000001</v>
+      </c>
+      <c r="AE7">
+        <v>69.036000000000001</v>
+      </c>
+      <c r="AF7">
+        <v>232.89099999999999</v>
+      </c>
+      <c r="AG7">
+        <v>687.45899999999995</v>
+      </c>
+      <c r="AH7">
+        <v>473.98899999999998</v>
+      </c>
+      <c r="AI7">
+        <v>106.17700000000001</v>
+      </c>
+      <c r="AJ7">
+        <v>163.05799999999999</v>
+      </c>
+      <c r="AK7">
+        <v>11.952999999999999</v>
+      </c>
+      <c r="AL7">
+        <v>9.4239999999999995</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>12.124000000000001</v>
+      </c>
+      <c r="AP7">
+        <v>31.38</v>
+      </c>
+      <c r="AQ7">
+        <v>10.609</v>
+      </c>
+      <c r="AR7">
+        <v>106.628</v>
+      </c>
+      <c r="AS7">
+        <v>5.5970000000000004</v>
+      </c>
+      <c r="AT7">
+        <v>114.511</v>
+      </c>
+      <c r="AU7">
+        <v>27.88</v>
+      </c>
+      <c r="AV7">
+        <v>402.46199999999999</v>
+      </c>
+      <c r="AW7">
+        <v>89.424000000000007</v>
+      </c>
+      <c r="AX7">
+        <v>17.79</v>
+      </c>
+      <c r="AY7">
+        <v>0</v>
+      </c>
+      <c r="AZ7">
+        <v>0</v>
+      </c>
+      <c r="BA7">
+        <v>0</v>
+      </c>
+      <c r="BB7">
+        <v>2.5920000000000001</v>
+      </c>
+      <c r="BC7">
+        <v>50.877899999999997</v>
+      </c>
+      <c r="BD7">
+        <v>118.012</v>
+      </c>
+      <c r="BE7">
+        <v>205.17599999999999</v>
+      </c>
+      <c r="BF7">
+        <v>250.03700000000001</v>
+      </c>
+      <c r="BG7">
+        <v>57.329700000000003</v>
+      </c>
+      <c r="BH7">
+        <v>228.70699999999999</v>
+      </c>
+      <c r="BI7">
+        <v>75.908100000000005</v>
+      </c>
+      <c r="BJ7">
+        <v>31.494499999999999</v>
+      </c>
+      <c r="BK7">
+        <v>10.197699999999999</v>
+      </c>
+      <c r="BL7">
+        <v>0</v>
+      </c>
+      <c r="BM7">
+        <v>0</v>
+      </c>
+      <c r="BN7">
+        <v>1.0299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8">
+        <v>-118.690808</v>
+      </c>
+      <c r="E8">
+        <v>36.712986999999998</v>
+      </c>
+      <c r="F8">
+        <v>49.804000000000002</v>
+      </c>
+      <c r="G8">
+        <v>46.280500000000004</v>
+      </c>
+      <c r="H8">
+        <v>204.47499999999999</v>
+      </c>
+      <c r="I8">
+        <v>635.40300000000002</v>
+      </c>
+      <c r="J8">
+        <v>312.79199999999997</v>
+      </c>
+      <c r="K8">
+        <v>87.760800000000003</v>
+      </c>
+      <c r="L8">
+        <v>108.48399999999999</v>
+      </c>
+      <c r="M8">
+        <v>16.154900000000001</v>
+      </c>
+      <c r="N8">
+        <v>7.7763</v>
+      </c>
+      <c r="O8">
+        <v>1.45299</v>
+      </c>
+      <c r="P8">
+        <v>6.4841600000000001</v>
+      </c>
+      <c r="Q8">
+        <v>14.228300000000001</v>
+      </c>
+      <c r="R8">
+        <v>3.06881</v>
+      </c>
+      <c r="S8">
+        <v>81.471100000000007</v>
+      </c>
+      <c r="T8">
+        <v>3.2578999999999998</v>
+      </c>
+      <c r="U8">
+        <v>89.351900000000001</v>
+      </c>
+      <c r="V8">
+        <v>22.6691</v>
+      </c>
+      <c r="W8">
+        <v>346.09899999999999</v>
+      </c>
+      <c r="X8">
+        <v>81.267200000000003</v>
+      </c>
+      <c r="Y8">
+        <v>13.692</v>
+      </c>
+      <c r="Z8">
+        <v>0.43120900000000001</v>
+      </c>
+      <c r="AA8">
+        <v>18.094899999999999</v>
+      </c>
+      <c r="AB8">
+        <v>2.6359599999999999</v>
+      </c>
+      <c r="AC8">
+        <v>10.493499999999999</v>
+      </c>
+      <c r="AD8">
+        <v>62.883000000000003</v>
+      </c>
+      <c r="AE8">
+        <v>45.643000000000001</v>
+      </c>
+      <c r="AF8">
+        <v>199.959</v>
+      </c>
+      <c r="AG8">
+        <v>633.29499999999996</v>
+      </c>
+      <c r="AH8">
+        <v>307.04000000000002</v>
+      </c>
+      <c r="AI8">
+        <v>87.674000000000007</v>
+      </c>
+      <c r="AJ8">
+        <v>111.732</v>
+      </c>
+      <c r="AK8">
+        <v>16.295000000000002</v>
+      </c>
+      <c r="AL8">
+        <v>7.6680000000000001</v>
+      </c>
+      <c r="AM8">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="AN8">
+        <v>6.742</v>
+      </c>
+      <c r="AP8">
+        <v>15.343999999999999</v>
+      </c>
+      <c r="AQ8">
+        <v>3.887</v>
+      </c>
+      <c r="AR8">
+        <v>79.441000000000003</v>
+      </c>
+      <c r="AS8">
+        <v>3.26</v>
+      </c>
+      <c r="AT8">
+        <v>88.853999999999999</v>
+      </c>
+      <c r="AU8">
+        <v>21.792000000000002</v>
+      </c>
+      <c r="AV8">
+        <v>347.05399999999997</v>
+      </c>
+      <c r="AW8">
+        <v>81.98</v>
+      </c>
+      <c r="AX8">
+        <v>9.9359999999999999</v>
+      </c>
+      <c r="AY8">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="AZ8">
+        <v>16.384</v>
+      </c>
+      <c r="BA8">
+        <v>2.5449999999999999</v>
+      </c>
+      <c r="BB8">
+        <v>10.718999999999999</v>
+      </c>
+      <c r="BC8">
+        <v>43.702300000000001</v>
+      </c>
+      <c r="BD8">
+        <v>112.086</v>
+      </c>
+      <c r="BE8">
+        <v>152.78</v>
+      </c>
+      <c r="BF8">
+        <v>204.16399999999999</v>
+      </c>
+      <c r="BG8">
+        <v>92.772999999999996</v>
+      </c>
+      <c r="BH8">
+        <v>141.74600000000001</v>
+      </c>
+      <c r="BI8">
+        <v>63.175800000000002</v>
+      </c>
+      <c r="BJ8">
+        <v>23.820900000000002</v>
+      </c>
+      <c r="BK8">
+        <v>6.8852900000000004</v>
+      </c>
+      <c r="BL8">
+        <v>0</v>
+      </c>
+      <c r="BM8">
+        <v>0.54130800000000001</v>
+      </c>
+      <c r="BN8">
+        <v>1.2849699999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>-9999</v>
+      </c>
+      <c r="G9">
+        <v>-9999</v>
+      </c>
+      <c r="H9">
+        <v>-9999</v>
+      </c>
+      <c r="I9">
+        <v>-9999</v>
+      </c>
+      <c r="J9">
+        <v>-9999</v>
+      </c>
+      <c r="K9">
+        <v>-9999</v>
+      </c>
+      <c r="L9">
+        <v>-9999</v>
+      </c>
+      <c r="M9">
+        <v>-9999</v>
+      </c>
+      <c r="N9">
+        <v>-9999</v>
+      </c>
+      <c r="O9">
+        <v>-9999</v>
+      </c>
+      <c r="P9">
+        <v>-9999</v>
+      </c>
+      <c r="Q9">
+        <v>-9999</v>
+      </c>
+      <c r="R9">
+        <v>-9999</v>
+      </c>
+      <c r="S9">
+        <v>-9999</v>
+      </c>
+      <c r="T9">
+        <v>-9999</v>
+      </c>
+      <c r="U9">
+        <v>-9999</v>
+      </c>
+      <c r="V9">
+        <v>-9999</v>
+      </c>
+      <c r="W9">
+        <v>-9999</v>
+      </c>
+      <c r="X9">
+        <v>-9999</v>
+      </c>
+      <c r="Y9">
+        <v>-9999</v>
+      </c>
+      <c r="Z9">
+        <v>-9999</v>
+      </c>
+      <c r="AA9">
+        <v>-9999</v>
+      </c>
+      <c r="AB9">
+        <v>-9999</v>
+      </c>
+      <c r="AC9">
+        <v>-9999</v>
+      </c>
+      <c r="AD9">
+        <v>-9999</v>
+      </c>
+      <c r="AE9">
+        <v>-9999</v>
+      </c>
+      <c r="AF9">
+        <v>-9999</v>
+      </c>
+      <c r="AG9">
+        <v>-9999</v>
+      </c>
+      <c r="AH9">
+        <v>-9999</v>
+      </c>
+      <c r="AI9">
+        <v>-9999</v>
+      </c>
+      <c r="AJ9">
+        <v>-9999</v>
+      </c>
+      <c r="AK9">
+        <v>-9999</v>
+      </c>
+      <c r="AL9">
+        <v>-9999</v>
+      </c>
+      <c r="AM9">
+        <v>-9999</v>
+      </c>
+      <c r="AN9">
+        <v>-9999</v>
+      </c>
+      <c r="AP9">
+        <v>-9999</v>
+      </c>
+      <c r="AQ9">
+        <v>-9999</v>
+      </c>
+      <c r="AR9">
+        <v>-9999</v>
+      </c>
+      <c r="AS9">
+        <v>-9999</v>
+      </c>
+      <c r="AT9">
+        <v>-9999</v>
+      </c>
+      <c r="AU9">
+        <v>-9999</v>
+      </c>
+      <c r="AV9">
+        <v>-9999</v>
+      </c>
+      <c r="AW9">
+        <v>-9999</v>
+      </c>
+      <c r="AX9">
+        <v>-9999</v>
+      </c>
+      <c r="AY9">
+        <v>-9999</v>
+      </c>
+      <c r="AZ9">
+        <v>-9999</v>
+      </c>
+      <c r="BA9">
+        <v>-9999</v>
+      </c>
+      <c r="BB9">
+        <v>-9999</v>
+      </c>
+      <c r="BC9">
+        <v>-9999</v>
+      </c>
+      <c r="BD9">
+        <v>-9999</v>
+      </c>
+      <c r="BE9">
+        <v>-9999</v>
+      </c>
+      <c r="BF9">
+        <v>-9999</v>
+      </c>
+      <c r="BG9">
+        <v>-9999</v>
+      </c>
+      <c r="BH9">
+        <v>-9999</v>
+      </c>
+      <c r="BI9">
+        <v>-9999</v>
+      </c>
+      <c r="BJ9">
+        <v>-9999</v>
+      </c>
+      <c r="BK9">
+        <v>-9999</v>
+      </c>
+      <c r="BL9">
+        <v>-9999</v>
+      </c>
+      <c r="BM9">
+        <v>-9999</v>
+      </c>
+      <c r="BN9">
+        <v>-9999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>